<commit_message>
Publish SMART IG v2.0.0-rc2
</commit_message>
<xml_diff>
--- a/fhir/finnish-smart/StructureDefinition-fi-smart-allergy-intolerance.xlsx
+++ b/fhir/finnish-smart/StructureDefinition-fi-smart-allergy-intolerance.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-rc1</t>
+    <t>2.0.0-rc2</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-06T22:29:11+02:00</t>
+    <t>2025-05-11T17:07:13+03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1355,17 +1355,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="41.68359375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="41.68359375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.3515625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.1484375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.7109375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="12.1875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="35.95703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="35.95703125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="9.79296875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="33.17578125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.30078125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="3.953125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.265625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="12.6875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="10.51171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="55.890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="48.2109375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1374,25 +1374,25 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.04296875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.77734375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.13671875" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="120.9609375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="59.3125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="15.703125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="13.125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="38.89453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.53125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="7.80078125" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="13.609375" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="13.91796875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="15.01171875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="14.62890625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="104.34375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="51.1640625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.07421875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="17.98046875" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="16.2578125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="13.54296875" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="11.3203125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="33.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="8.22265625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="8.53125" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="37" max="37" width="255.0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="33.05078125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="40.33203125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="28.5078125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="34.7890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>